<commit_message>
almost done the report
</commit_message>
<xml_diff>
--- a/Report/Data Dictionary/Data Dictionary.xlsx
+++ b/Report/Data Dictionary/Data Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100624914\Documents\Capstone\capstone\Report\Data Dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkfenix\Documents\School\Year_3\Semester_2\CAPSTONE\capstone\Report\Data Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609E87A9-8949-4AC4-9F8B-A6C9AEB87AEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2CACB3-E1E1-4A0D-9E01-8F4503840CB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7050301C-00A8-4ED2-83D6-B0D265C97AB4}"/>
+    <workbookView xWindow="-4665" yWindow="2340" windowWidth="9405" windowHeight="12240" xr2:uid="{7050301C-00A8-4ED2-83D6-B0D265C97AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="105">
   <si>
     <t>Table</t>
   </si>
@@ -748,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE4A736-45F7-4D2E-94A4-ECF8FBE25729}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="M103" sqref="M103"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,691 +1208,695 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6" t="s">
+      <c r="D29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="G29" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="D30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="F30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="D31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="F31" s="6"/>
+      <c r="G31" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="D32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="D33" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+      <c r="F33" s="6"/>
+      <c r="G33" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+      <c r="D34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
+      <c r="D35" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4" t="s">
+      <c r="D40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6" t="s">
+      <c r="D41" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+      <c r="G41" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="D42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+      <c r="F42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="D43" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
+      <c r="F43" s="6"/>
+      <c r="G43" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="D44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
+      <c r="F44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
+      <c r="G46" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6" t="s">
+      <c r="D47" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
+      <c r="G47" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4" t="s">
+      <c r="D48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
+      <c r="G48" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6" t="s">
+      <c r="D49" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="3" t="s">
+      <c r="G49" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="s">
+      <c r="D50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6" t="s">
+      <c r="D51" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G50" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
+      <c r="G51" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
+      <c r="D52" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
+      <c r="D53" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4" t="s">
+      <c r="D54" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G53" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
+      <c r="G54" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" s="6" t="s">
+      <c r="D55" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="3" t="s">
+      <c r="F55" s="6"/>
+      <c r="G55" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="D56" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
+      <c r="F56" s="4"/>
+      <c r="G56" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="5" t="s">
+      <c r="D58" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" s="6" t="s">
+      <c r="D59" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
+      <c r="F59" s="6"/>
+      <c r="G59" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D61" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4" t="s">
+      <c r="D62" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
+      <c r="G62" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="3" t="s">
+      <c r="D63" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
+      <c r="D64" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
+      <c r="G64" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="D65" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="G67" s="4" t="s">
         <v>87</v>
       </c>
@@ -1902,15 +1906,15 @@
         <v>64</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="E68" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F68" s="6"/>
       <c r="G68" s="6" t="s">
         <v>87</v>
       </c>
@@ -1920,15 +1924,17 @@
         <v>64</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E69" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -1936,51 +1942,49 @@
         <v>64</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+      <c r="F70" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="G70" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E71" s="4"/>
-      <c r="F71" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="F71" s="4"/>
       <c r="G71" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E72" s="6"/>
-      <c r="F72" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="F72" s="6"/>
       <c r="G72" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -1988,7 +1992,7 @@
         <v>69</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>90</v>
@@ -2006,13 +2010,15 @@
         <v>69</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
+      <c r="F74" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="G74" s="6" t="s">
         <v>87</v>
       </c>
@@ -2022,41 +2028,41 @@
         <v>69</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
+      <c r="F75" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="G75" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>89</v>
       </c>
       <c r="E76" s="6"/>
-      <c r="F76" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="F76" s="6"/>
       <c r="G76" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>89</v>
@@ -2072,15 +2078,17 @@
         <v>75</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>89</v>
       </c>
       <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
+      <c r="F78" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="G78" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2088,7 +2096,7 @@
         <v>75</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>89</v>
@@ -2104,7 +2112,7 @@
         <v>75</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>89</v>
@@ -2112,7 +2120,7 @@
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -2120,7 +2128,7 @@
         <v>75</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>89</v>
@@ -2136,7 +2144,7 @@
         <v>75</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>89</v>
@@ -2149,35 +2157,31 @@
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E83" s="4"/>
-      <c r="F83" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="F83" s="4"/>
       <c r="G83" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>102</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E84" s="6"/>
       <c r="F84" s="6"/>
       <c r="G84" s="6" t="s">
         <v>87</v>
@@ -2188,15 +2192,15 @@
         <v>80</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E85" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="G85" s="4" t="s">
         <v>87</v>
       </c>
@@ -2206,12 +2210,14 @@
         <v>80</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E86" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="F86" s="6"/>
       <c r="G86" s="6" t="s">
         <v>87</v>
@@ -2222,12 +2228,14 @@
         <v>80</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E87" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4" t="s">
         <v>87</v>
@@ -2238,10 +2246,10 @@
         <v>80</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
@@ -2251,35 +2259,31 @@
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E89" s="4"/>
-      <c r="F89" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="F89" s="4"/>
       <c r="G89" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>102</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E90" s="6"/>
       <c r="F90" s="6"/>
       <c r="G90" s="6" t="s">
         <v>87</v>
@@ -2290,13 +2294,15 @@
         <v>84</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
+      <c r="F91" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="G91" s="4" t="s">
         <v>87</v>
       </c>
@@ -2306,24 +2312,58 @@
         <v>84</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B130" s="5"/>
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>